<commit_message>
new table in datacreation
</commit_message>
<xml_diff>
--- a/yes-genie-testautomation-GenieDataCreation/src/main/resources/kpi.xlsx
+++ b/yes-genie-testautomation-GenieDataCreation/src/main/resources/kpi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AUS_MASTER" sheetId="1" state="visible" r:id="rId2"/>
@@ -441,10 +441,10 @@
     <t xml:space="preserve">998003452_CB</t>
   </si>
   <si>
-    <t xml:space="preserve">KPI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI Value</t>
+    <t xml:space="preserve">kpi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kpi_value</t>
   </si>
   <si>
     <t xml:space="preserve">996264849_PPI</t>
@@ -482,11 +482,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D\-MMM\-YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -509,12 +510,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -588,7 +583,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -625,10 +620,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -637,7 +628,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -709,29 +700,29 @@
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="4.59183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="30.8673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="7.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.9030612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2091836734694"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.5051020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.969387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="19.3826530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="48.5357142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="98.7857142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="20.25"/>
-    <col collapsed="false" hidden="false" max="257" min="16" style="1" width="11.484693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.484693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="30.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="38.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="48.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="98.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="20.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="16" style="1" width="11.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="11.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -887,7 +878,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -902,24 +893,24 @@
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B44" activeCellId="0" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.75"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.5"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.9234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.3826530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.0765306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6275510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="16.6479591836735"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="19.2397959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.0612244897959"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="1" width="8.70918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="8.70918367346939"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="16.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="257" min="12" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="258" style="0" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,7 +2491,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2515,18 +2506,17 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="31.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="22.9234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="22.2295918367347"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="258" style="0" width="11.5663265306122"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="22.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="7" width="22.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="257" min="5" style="7" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2603,7 +2593,7 @@
       <c r="A6" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="4" t="n">
         <v>998003452</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -2617,7 +2607,7 @@
       <c r="A7" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="4" t="n">
         <v>998003452</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -2630,7 +2620,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>